<commit_message>
Updated arrays and strings
</commit_message>
<xml_diff>
--- a/Coder Army Sheet.xlsx
+++ b/Coder Army Sheet.xlsx
@@ -2734,11 +2734,11 @@
   </sheetPr>
   <dimension ref="A1:E746"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B68" activeCellId="0" sqref="B68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.88"/>
@@ -2992,7 +2992,7 @@
         <v>3</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3043,7 +3043,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3077,7 +3077,7 @@
         <v>5</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3434,7 +3434,7 @@
         <v>11</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3866,7 +3866,7 @@
         <v>20</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Arrays and Strings updated
</commit_message>
<xml_diff>
--- a/Coder Army Sheet.xlsx
+++ b/Coder Army Sheet.xlsx
@@ -2734,11 +2734,11 @@
   </sheetPr>
   <dimension ref="A1:E746"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B65" activeCellId="0" sqref="B65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.88"/>
@@ -3264,7 +3264,7 @@
         <v>7</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3366,7 +3366,7 @@
         <v>9</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3781,7 +3781,7 @@
         <v>18</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3815,7 +3815,7 @@
         <v>18</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Arrays and Searching updated
</commit_message>
<xml_diff>
--- a/Coder Army Sheet.xlsx
+++ b/Coder Army Sheet.xlsx
@@ -2734,11 +2734,11 @@
   </sheetPr>
   <dimension ref="A1:E746"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A104" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E130" activeCellId="0" sqref="E130"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B110" activeCellId="0" sqref="B110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.88"/>
@@ -4468,7 +4468,7 @@
         <v>32</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4502,7 +4502,7 @@
         <v>32</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4553,7 +4553,7 @@
         <v>33</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4570,7 +4570,7 @@
         <v>33</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4587,7 +4587,7 @@
         <v>34</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Stacks and queues updated
</commit_message>
<xml_diff>
--- a/Coder Army Sheet.xlsx
+++ b/Coder Army Sheet.xlsx
@@ -3687,8 +3687,8 @@
   <sheetPr/>
   <dimension ref="A1:F746"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="E239" sqref="E239"/>
+    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
+      <selection activeCell="B277" sqref="B277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5462962962963" defaultRowHeight="13.2" outlineLevelCol="5"/>
@@ -8225,7 +8225,7 @@
         <v>84</v>
       </c>
       <c r="E270" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="271" ht="15.6" spans="1:5">
@@ -8242,7 +8242,7 @@
         <v>85</v>
       </c>
       <c r="E271" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="272" ht="15.6" spans="1:5">
@@ -8327,7 +8327,7 @@
         <v>86</v>
       </c>
       <c r="E276" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="277" ht="15.6" spans="1:5">

</xml_diff>

<commit_message>
Stacks and trees updated
</commit_message>
<xml_diff>
--- a/Coder Army Sheet.xlsx
+++ b/Coder Army Sheet.xlsx
@@ -3687,8 +3687,8 @@
   <sheetPr/>
   <dimension ref="A1:F746"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A304" workbookViewId="0">
-      <selection activeCell="E316" sqref="E316"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A284" workbookViewId="0">
+      <selection activeCell="E298" sqref="E298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5462962962963" defaultRowHeight="13.2" outlineLevelCol="5"/>
@@ -7742,7 +7742,7 @@
         <v>74</v>
       </c>
       <c r="E241" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="242" ht="15.6" spans="1:5">
@@ -7895,7 +7895,7 @@
         <v>78</v>
       </c>
       <c r="E250" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="251" ht="15.6" spans="1:5">
@@ -8657,7 +8657,7 @@
         <v>92</v>
       </c>
       <c r="E296" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="297" ht="15.6" spans="1:5">
@@ -8691,7 +8691,7 @@
         <v>93</v>
       </c>
       <c r="E298" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="299" ht="15.6" spans="1:5">

</xml_diff>

<commit_message>
Bst and heaps added
</commit_message>
<xml_diff>
--- a/Coder Army Sheet.xlsx
+++ b/Coder Army Sheet.xlsx
@@ -3687,8 +3687,8 @@
   <sheetPr/>
   <dimension ref="A1:F746"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A284" workbookViewId="0">
-      <selection activeCell="E298" sqref="E298"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A322" workbookViewId="0">
+      <selection activeCell="E334" sqref="E334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5462962962963" defaultRowHeight="13.2" outlineLevelCol="5"/>
@@ -9445,7 +9445,7 @@
         <v>108</v>
       </c>
       <c r="E343" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="344" ht="15.6" spans="1:5">
@@ -9462,7 +9462,7 @@
         <v>108</v>
       </c>
       <c r="E344" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="345" ht="15.6" spans="1:5">
@@ -9530,7 +9530,7 @@
         <v>109</v>
       </c>
       <c r="E348" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="349" ht="15.6" spans="1:5">
@@ -10233,7 +10233,7 @@
         <v>121</v>
       </c>
       <c r="E390" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="391" ht="15.6" spans="1:5">
@@ -10250,7 +10250,7 @@
         <v>121</v>
       </c>
       <c r="E391" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="392" ht="15.6" spans="1:5">
@@ -10488,7 +10488,7 @@
         <v>125</v>
       </c>
       <c r="E405" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="406" ht="15.6" spans="1:5">

</xml_diff>

<commit_message>
Greedy and DP updated
</commit_message>
<xml_diff>
--- a/Coder Army Sheet.xlsx
+++ b/Coder Army Sheet.xlsx
@@ -3687,8 +3687,8 @@
   <sheetPr/>
   <dimension ref="A1:F746"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A513" workbookViewId="0">
-      <selection activeCell="B520" sqref="B520"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="F115" sqref="F115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5462962962963" defaultRowHeight="13.2" outlineLevelCol="5"/>
@@ -10851,7 +10851,7 @@
         <v>133</v>
       </c>
       <c r="E427" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="428" ht="15.6" spans="1:5">
@@ -11996,7 +11996,7 @@
         <v>155</v>
       </c>
       <c r="E495" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="496" ht="15.6" spans="1:5">
@@ -13646,7 +13646,7 @@
         <v>188</v>
       </c>
       <c r="E594" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="595" ht="15.6" spans="1:5">
@@ -13680,7 +13680,7 @@
         <v>188</v>
       </c>
       <c r="E596" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="597" ht="15.6" spans="1:5">

</xml_diff>

<commit_message>
Hashing and DP updated
</commit_message>
<xml_diff>
--- a/Coder Army Sheet.xlsx
+++ b/Coder Army Sheet.xlsx
@@ -3687,8 +3687,8 @@
   <sheetPr/>
   <dimension ref="A1:F746"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A627" workbookViewId="0">
-      <selection activeCell="B635" sqref="B635"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5462962962963" defaultRowHeight="13.2" outlineLevelCol="5"/>
@@ -12223,7 +12223,7 @@
         <v>159</v>
       </c>
       <c r="E509" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="510" ht="15.6" spans="1:5">
@@ -12257,7 +12257,7 @@
         <v>159</v>
       </c>
       <c r="E511" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="512" ht="15.6" spans="1:5">
@@ -13714,7 +13714,7 @@
         <v>189</v>
       </c>
       <c r="E598" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="599" ht="15.6" spans="1:5">
@@ -13833,7 +13833,7 @@
         <v>191</v>
       </c>
       <c r="E605" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="606" ht="15.6" spans="1:5">
@@ -14292,7 +14292,7 @@
         <v>200</v>
       </c>
       <c r="E632" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="633" ht="15.6" spans="1:5">

</xml_diff>

<commit_message>
Searching and Sorting updated
</commit_message>
<xml_diff>
--- a/Coder Army Sheet.xlsx
+++ b/Coder Army Sheet.xlsx
@@ -3687,8 +3687,8 @@
   <sheetPr/>
   <dimension ref="A1:F746"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="B232" sqref="B232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5462962962963" defaultRowHeight="13.2" outlineLevelCol="5"/>
@@ -5447,7 +5447,7 @@
         <v>32</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106" ht="15.6" spans="1:5">
@@ -5906,7 +5906,7 @@
         <v>40</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F132" s="2"/>
     </row>

</xml_diff>

<commit_message>
Strings and queue updated
</commit_message>
<xml_diff>
--- a/Coder Army Sheet.xlsx
+++ b/Coder Army Sheet.xlsx
@@ -3687,8 +3687,8 @@
   <sheetPr/>
   <dimension ref="A1:F746"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A381" workbookViewId="0">
-      <selection activeCell="B392" sqref="B392"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A463" workbookViewId="0">
+      <selection activeCell="B475" sqref="B475"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5462962962963" defaultRowHeight="13.2" outlineLevelCol="5"/>
@@ -4686,7 +4686,7 @@
         <v>17</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" ht="15.6" spans="1:5">
@@ -8151,7 +8151,7 @@
         <v>83</v>
       </c>
       <c r="E266" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="267" ht="15.6" spans="1:5">

</xml_diff>

<commit_message>
Updated stack and queue
</commit_message>
<xml_diff>
--- a/Coder Army Sheet.xlsx
+++ b/Coder Army Sheet.xlsx
@@ -3700,8 +3700,8 @@
   <sheetPr/>
   <dimension ref="A1:F746"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A473" workbookViewId="0">
-      <selection activeCell="B478" sqref="B478"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A271" workbookViewId="0">
+      <selection activeCell="C280" sqref="C280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5462962962963" defaultRowHeight="13.2" outlineLevelCol="5"/>
@@ -4181,7 +4181,7 @@
         <v>7</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" ht="15.6" spans="1:5">
@@ -8385,7 +8385,7 @@
         <v>88</v>
       </c>
       <c r="E279" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="280" ht="15.6" spans="1:5">

</xml_diff>

<commit_message>
Searching and trees updated
</commit_message>
<xml_diff>
--- a/Coder Army Sheet.xlsx
+++ b/Coder Army Sheet.xlsx
@@ -3700,8 +3700,8 @@
   <sheetPr/>
   <dimension ref="A1:F746"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A271" workbookViewId="0">
-      <selection activeCell="C280" sqref="C280"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A291" workbookViewId="0">
+      <selection activeCell="E308" sqref="E308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5462962962963" defaultRowHeight="13.2" outlineLevelCol="5"/>
@@ -5777,7 +5777,7 @@
         <v>37</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125" ht="15.6" spans="1:5">
@@ -8868,7 +8868,7 @@
         <v>95</v>
       </c>
       <c r="E308" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="309" ht="15.6" spans="1:5">

</xml_diff>

<commit_message>
Binary Search tree updated
</commit_message>
<xml_diff>
--- a/Coder Army Sheet.xlsx
+++ b/Coder Army Sheet.xlsx
@@ -3700,8 +3700,8 @@
   <sheetPr/>
   <dimension ref="A1:F746"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A311" workbookViewId="0">
-      <selection activeCell="B330" sqref="B330"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A355" workbookViewId="0">
+      <selection activeCell="E361" sqref="E361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5462962962963" defaultRowHeight="13.2" outlineLevelCol="5"/>
@@ -9758,7 +9758,7 @@
         <v>112</v>
       </c>
       <c r="E361" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="362" ht="15.6" spans="1:5">
@@ -9996,7 +9996,7 @@
         <v>117</v>
       </c>
       <c r="E375" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="376" ht="15.6" spans="1:5">
@@ -10064,7 +10064,7 @@
         <v>118</v>
       </c>
       <c r="E379" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="380" ht="15.6" spans="1:5">

</xml_diff>